<commit_message>
Minor in data modelling
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_text.xlsx
+++ b/modeling/results/feature_imp_text.xlsx
@@ -28,298 +28,298 @@
     <t>aumento</t>
   </si>
   <si>
+    <t>xliii</t>
+  </si>
+  <si>
+    <t>concessão</t>
+  </si>
+  <si>
+    <t>ordem prisão</t>
+  </si>
+  <si>
+    <t>justiça indeferiu</t>
+  </si>
+  <si>
+    <t>julgado turma</t>
+  </si>
+  <si>
+    <t>arquivado</t>
+  </si>
+  <si>
+    <t>enunciado súmula</t>
+  </si>
+  <si>
+    <t>deferida</t>
+  </si>
+  <si>
+    <t>senha relatório</t>
+  </si>
+  <si>
+    <t>concessão ordem</t>
+  </si>
+  <si>
+    <t>outro motivo</t>
+  </si>
+  <si>
+    <t>liberdade provisória</t>
+  </si>
+  <si>
+    <t>assessoria</t>
+  </si>
+  <si>
+    <t>implicou deferimento</t>
+  </si>
+  <si>
+    <t>deferido</t>
+  </si>
+  <si>
+    <t>liminar espécie</t>
+  </si>
+  <si>
+    <t>stj indeferiu</t>
+  </si>
+  <si>
+    <t>liminar hc</t>
+  </si>
+  <si>
     <t>deferi</t>
   </si>
   <si>
-    <t>deferimento</t>
+    <t>relatório http</t>
+  </si>
+  <si>
+    <t>restritiva direitos</t>
+  </si>
+  <si>
+    <t>manifesta ilegalidade</t>
+  </si>
+  <si>
+    <t>opina deferimento</t>
+  </si>
+  <si>
+    <t>restritiva</t>
+  </si>
+  <si>
+    <t>informado</t>
+  </si>
+  <si>
+    <t>http sob</t>
+  </si>
+  <si>
+    <t>inconstitucional</t>
+  </si>
+  <si>
+    <t>provisória formulado</t>
+  </si>
+  <si>
+    <t>cautelar pois</t>
+  </si>
+  <si>
+    <t>proferida ministro</t>
+  </si>
+  <si>
+    <t>preventiva fundamentos</t>
+  </si>
+  <si>
+    <t>tutela cautelar</t>
+  </si>
+  <si>
+    <t>fundamentos insubsistência</t>
+  </si>
+  <si>
+    <t>liminar suspender</t>
+  </si>
+  <si>
+    <t>lxi</t>
+  </si>
+  <si>
+    <t>opinou concessão</t>
+  </si>
+  <si>
+    <t>arquivado definitivo</t>
+  </si>
+  <si>
+    <t>república concessão</t>
+  </si>
+  <si>
+    <t>gabinete prestou</t>
+  </si>
+  <si>
+    <t>formalizado ato</t>
   </si>
   <si>
     <t>deferimento liminar</t>
   </si>
   <si>
-    <t>outro motivo</t>
-  </si>
-  <si>
-    <t>senha relatório</t>
-  </si>
-  <si>
-    <t>referida decisão</t>
-  </si>
-  <si>
-    <t>relatório http</t>
-  </si>
-  <si>
-    <t>cpp art</t>
-  </si>
-  <si>
-    <t>deferida</t>
-  </si>
-  <si>
-    <t>decretada desfavor</t>
-  </si>
-  <si>
-    <t>ordem prisão</t>
-  </si>
-  <si>
-    <t>manifesta</t>
-  </si>
-  <si>
-    <t>liminar hc</t>
-  </si>
-  <si>
-    <t>julgado turma</t>
-  </si>
-  <si>
-    <t>stj indeferiu</t>
-  </si>
-  <si>
-    <t>substituir</t>
+    <t>deferida assessoria</t>
+  </si>
+  <si>
+    <t>deferi pedido</t>
+  </si>
+  <si>
+    <t>sobrestamento</t>
+  </si>
+  <si>
+    <t>código senha</t>
+  </si>
+  <si>
+    <t>contornos impetração</t>
+  </si>
+  <si>
+    <t>desta suprema</t>
+  </si>
+  <si>
+    <t>definitivo após</t>
+  </si>
+  <si>
+    <t>efêmero</t>
+  </si>
+  <si>
+    <t>resumida prisão</t>
+  </si>
+  <si>
+    <t>senha primeira</t>
+  </si>
+  <si>
+    <t>benefício liberdade</t>
+  </si>
+  <si>
+    <t>ficou</t>
+  </si>
+  <si>
+    <t>flagrante tráfico</t>
+  </si>
+  <si>
+    <t>sob código</t>
+  </si>
+  <si>
+    <t>precário</t>
+  </si>
+  <si>
+    <t>pertence grifei</t>
+  </si>
+  <si>
+    <t>precário efêmero</t>
+  </si>
+  <si>
+    <t>suspender efeitos</t>
+  </si>
+  <si>
+    <t>sistema jurídico</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>princípio liberdade</t>
+  </si>
+  <si>
+    <t>rtj rel</t>
+  </si>
+  <si>
+    <t>processo formalizado</t>
+  </si>
+  <si>
+    <t>revelou contornos</t>
+  </si>
+  <si>
+    <t>punir</t>
+  </si>
+  <si>
+    <t>suspender</t>
+  </si>
+  <si>
+    <t>paulo indeferiu</t>
+  </si>
+  <si>
+    <t>resumida</t>
+  </si>
+  <si>
+    <t>análise pedido</t>
+  </si>
+  <si>
+    <t>mendes hc</t>
+  </si>
+  <si>
+    <t>liminar deferida</t>
+  </si>
+  <si>
+    <t>art lvii</t>
+  </si>
+  <si>
+    <t>art lxi</t>
+  </si>
+  <si>
+    <t>assessoria prestou</t>
+  </si>
+  <si>
+    <t>assim resumida</t>
+  </si>
+  <si>
+    <t>assim revelou</t>
+  </si>
+  <si>
+    <t>aurélio decisão</t>
+  </si>
+  <si>
+    <t>campo precário</t>
+  </si>
+  <si>
+    <t>condenação penal</t>
+  </si>
+  <si>
+    <t>constitucional cf</t>
+  </si>
+  <si>
+    <t>defiro</t>
+  </si>
+  <si>
+    <t>deserção</t>
+  </si>
+  <si>
+    <t>efeitos ordem</t>
+  </si>
+  <si>
+    <t>eis informado</t>
+  </si>
+  <si>
+    <t>espécie ficou</t>
+  </si>
+  <si>
+    <t>fiança</t>
+  </si>
+  <si>
+    <t>ficou assim</t>
   </si>
   <si>
     <t>http</t>
   </si>
   <si>
-    <t>arquivado</t>
-  </si>
-  <si>
-    <t>liminar suspender</t>
-  </si>
-  <si>
-    <t>liminar espécie</t>
-  </si>
-  <si>
-    <t>justiça nº</t>
-  </si>
-  <si>
-    <t>jurisprudenciais</t>
-  </si>
-  <si>
-    <t>ministro gilson</t>
-  </si>
-  <si>
-    <t>mulheres</t>
-  </si>
-  <si>
-    <t>informado</t>
+    <t>impetração eis</t>
+  </si>
+  <si>
+    <t>inciso xliii</t>
+  </si>
+  <si>
+    <t>indefiro pedido</t>
+  </si>
+  <si>
+    <t>infligir</t>
+  </si>
+  <si>
+    <t>infligir punição</t>
+  </si>
+  <si>
+    <t>informado análise</t>
+  </si>
+  <si>
+    <t>instituto prisão</t>
+  </si>
+  <si>
+    <t>irrecorrível</t>
   </si>
   <si>
     <t>indiciado réu</t>
-  </si>
-  <si>
-    <t>opina concessão</t>
-  </si>
-  <si>
-    <t>análise pedido</t>
-  </si>
-  <si>
-    <t>opina deferimento</t>
-  </si>
-  <si>
-    <t>opinou concessão</t>
-  </si>
-  <si>
-    <t>implicou deferimento</t>
-  </si>
-  <si>
-    <t>paciente decretada</t>
-  </si>
-  <si>
-    <t>proferida ministro</t>
-  </si>
-  <si>
-    <t>relativização</t>
-  </si>
-  <si>
-    <t>república concessão</t>
-  </si>
-  <si>
-    <t>restritiva direitos</t>
-  </si>
-  <si>
-    <t>resumida prisão</t>
-  </si>
-  <si>
-    <t>resumiu apreciou</t>
-  </si>
-  <si>
-    <t>senha</t>
-  </si>
-  <si>
-    <t>sob código</t>
-  </si>
-  <si>
-    <t>sobrestamento</t>
-  </si>
-  <si>
-    <t>suspender</t>
-  </si>
-  <si>
-    <t>tutela</t>
-  </si>
-  <si>
-    <t>indeferiu liminarmente</t>
-  </si>
-  <si>
-    <t>violência grave</t>
-  </si>
-  <si>
-    <t>concessão ordem</t>
-  </si>
-  <si>
-    <t>assim resumida</t>
-  </si>
-  <si>
-    <t>efêmero</t>
-  </si>
-  <si>
-    <t>brasília residência</t>
-  </si>
-  <si>
-    <t>deferi pedido</t>
-  </si>
-  <si>
-    <t>autorizado</t>
-  </si>
-  <si>
-    <t>código senha</t>
-  </si>
-  <si>
-    <t>contornos</t>
-  </si>
-  <si>
-    <t>cautelares previstas</t>
-  </si>
-  <si>
-    <t>assessoria</t>
-  </si>
-  <si>
-    <t>art lxi</t>
-  </si>
-  <si>
-    <t>circunstâncias favoráveis</t>
-  </si>
-  <si>
-    <t>arquivado definitivo</t>
-  </si>
-  <si>
-    <t>concessão</t>
-  </si>
-  <si>
-    <t>efeitos ordem</t>
-  </si>
-  <si>
-    <t>resumida</t>
-  </si>
-  <si>
-    <t>cautelar pois</t>
-  </si>
-  <si>
-    <t>cautelar penal</t>
-  </si>
-  <si>
-    <t>impetração eis</t>
-  </si>
-  <si>
-    <t>campo precário</t>
-  </si>
-  <si>
-    <t>princípio liberdade</t>
-  </si>
-  <si>
-    <t>rtj rel</t>
-  </si>
-  <si>
-    <t>senha primeira</t>
-  </si>
-  <si>
-    <t>aurélio decisão</t>
-  </si>
-  <si>
-    <t>assim revelou</t>
-  </si>
-  <si>
-    <t>assessoria prestou</t>
-  </si>
-  <si>
-    <t>suspender efeitos</t>
-  </si>
-  <si>
-    <t>tutela cautelar</t>
-  </si>
-  <si>
-    <t>revelou contornos</t>
-  </si>
-  <si>
-    <t>precário</t>
-  </si>
-  <si>
-    <t>preventiva fundamentos</t>
-  </si>
-  <si>
-    <t>ficou</t>
-  </si>
-  <si>
-    <t>infligir</t>
-  </si>
-  <si>
-    <t>apreciou presente</t>
-  </si>
-  <si>
-    <t>gabinete prestou</t>
-  </si>
-  <si>
-    <t>informado análise</t>
-  </si>
-  <si>
-    <t>informações paciente</t>
-  </si>
-  <si>
-    <t>instituto prisão</t>
-  </si>
-  <si>
-    <t>irrecorrível</t>
-  </si>
-  <si>
-    <t>fundamentos insubsistência</t>
-  </si>
-  <si>
-    <t>ficou assim</t>
-  </si>
-  <si>
-    <t>liminar deferida</t>
-  </si>
-  <si>
-    <t>precário efêmero</t>
-  </si>
-  <si>
-    <t>espécie ficou</t>
-  </si>
-  <si>
-    <t>enquanto medida</t>
-  </si>
-  <si>
-    <t>eis informado</t>
-  </si>
-  <si>
-    <t>deserção</t>
-  </si>
-  <si>
-    <t>natureza infração</t>
-  </si>
-  <si>
-    <t>deferida assessoria</t>
-  </si>
-  <si>
-    <t>contornos impetração</t>
-  </si>
-  <si>
-    <t>condenação penal</t>
-  </si>
-  <si>
-    <t>http sob</t>
-  </si>
-  <si>
-    <t>infligir punição</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -704,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -712,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -720,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -768,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -784,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -856,7 +856,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -864,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -872,7 +872,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -880,7 +880,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -888,7 +888,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -896,7 +896,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -904,7 +904,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1144,7 +1144,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1152,7 +1152,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1160,7 +1160,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1168,7 +1168,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1176,7 +1176,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1184,7 +1184,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">

</xml_diff>

<commit_message>
Adjustements in model selection
</commit_message>
<xml_diff>
--- a/modeling/results/feature_imp_text.xlsx
+++ b/modeling/results/feature_imp_text.xlsx
@@ -22,304 +22,304 @@
     <t>Importance</t>
   </si>
   <si>
+    <t>indeferiu</t>
+  </si>
+  <si>
+    <t>deferimento</t>
+  </si>
+  <si>
+    <t>concessão ordem</t>
+  </si>
+  <si>
+    <t>concessão</t>
+  </si>
+  <si>
+    <t>estado paulo</t>
+  </si>
+  <si>
+    <t>óbice</t>
+  </si>
+  <si>
+    <t>ordem prisão</t>
+  </si>
+  <si>
+    <t>deferida</t>
+  </si>
+  <si>
+    <t>inconstitucional</t>
+  </si>
+  <si>
+    <t>sobrestamento</t>
+  </si>
+  <si>
+    <t>senha relatório</t>
+  </si>
+  <si>
+    <t>liminar hc</t>
+  </si>
+  <si>
+    <t>deferi</t>
+  </si>
+  <si>
+    <t>relatório http</t>
+  </si>
+  <si>
+    <t>manifesta ilegalidade</t>
+  </si>
+  <si>
+    <t>liminar suspender</t>
+  </si>
+  <si>
+    <t>liminarmente pedido</t>
+  </si>
+  <si>
+    <t>liminar deferida</t>
+  </si>
+  <si>
+    <t>anotou</t>
+  </si>
+  <si>
+    <t>indeferiu liminarmente</t>
+  </si>
+  <si>
+    <t>opina concessão</t>
+  </si>
+  <si>
+    <t>anos dois</t>
+  </si>
+  <si>
+    <t>opina deferimento</t>
+  </si>
+  <si>
+    <t>opinou concessão</t>
+  </si>
+  <si>
+    <t>outro motivo</t>
+  </si>
+  <si>
+    <t>preventiva fundamentos</t>
+  </si>
+  <si>
+    <t>processo revelador</t>
+  </si>
+  <si>
+    <t>providência procuradoria</t>
+  </si>
+  <si>
+    <t>república concessão</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>stj indeferiu</t>
+  </si>
+  <si>
+    <t>substituir prisão</t>
+  </si>
+  <si>
+    <t>violência grave</t>
+  </si>
+  <si>
+    <t>xliii constituição</t>
+  </si>
+  <si>
+    <t>presa</t>
+  </si>
+  <si>
+    <t>justiça nº</t>
+  </si>
+  <si>
+    <t>contornos</t>
+  </si>
+  <si>
+    <t>cautelares previstas</t>
+  </si>
+  <si>
+    <t>deste habeas</t>
+  </si>
+  <si>
+    <t>deferimento liminar</t>
+  </si>
+  <si>
+    <t>causas aumento</t>
+  </si>
+  <si>
+    <t>ficou</t>
+  </si>
+  <si>
+    <t>enunciado súmula</t>
+  </si>
+  <si>
+    <t>campo precário</t>
+  </si>
+  <si>
+    <t>publiquem</t>
+  </si>
+  <si>
+    <t>colham</t>
+  </si>
+  <si>
+    <t>senha primeira</t>
+  </si>
+  <si>
+    <t>república parecer</t>
+  </si>
+  <si>
+    <t>resumida</t>
+  </si>
+  <si>
+    <t>resumida prisão</t>
+  </si>
+  <si>
+    <t>revelador</t>
+  </si>
+  <si>
+    <t>revelou contornos</t>
+  </si>
+  <si>
+    <t>proferida ministro</t>
+  </si>
+  <si>
+    <t>procuradoria geral</t>
+  </si>
+  <si>
+    <t>ficou assim</t>
+  </si>
+  <si>
+    <t>procuradoria</t>
+  </si>
+  <si>
+    <t>ser julgado</t>
+  </si>
+  <si>
+    <t>sob código</t>
+  </si>
+  <si>
+    <t>aurélio decisão</t>
+  </si>
+  <si>
+    <t>assim revelou</t>
+  </si>
+  <si>
+    <t>substituir</t>
+  </si>
+  <si>
+    <t>assim resumida</t>
+  </si>
+  <si>
+    <t>suspender</t>
+  </si>
+  <si>
+    <t>suspender efeitos</t>
+  </si>
+  <si>
+    <t>teixeira</t>
+  </si>
+  <si>
+    <t>vedação liberdade</t>
+  </si>
+  <si>
+    <t>assessoria prestou</t>
+  </si>
+  <si>
+    <t>assessoria</t>
+  </si>
+  <si>
+    <t>análise pedido</t>
+  </si>
+  <si>
+    <t>brasília residência</t>
+  </si>
+  <si>
+    <t>prestadas gabinete</t>
+  </si>
+  <si>
+    <t>colham parecer</t>
+  </si>
+  <si>
+    <t>liminar assessor</t>
+  </si>
+  <si>
+    <t>gabinete prestou</t>
+  </si>
+  <si>
+    <t>habeas contra</t>
+  </si>
+  <si>
+    <t>idêntica medida</t>
+  </si>
+  <si>
+    <t>impetração eis</t>
+  </si>
+  <si>
+    <t>implicou deferimento</t>
+  </si>
+  <si>
+    <t>espécie ficou</t>
+  </si>
+  <si>
+    <t>informado</t>
+  </si>
+  <si>
+    <t>informado análise</t>
+  </si>
+  <si>
+    <t>informações paciente</t>
+  </si>
+  <si>
+    <t>julgado turma</t>
+  </si>
+  <si>
+    <t>enunciado</t>
+  </si>
+  <si>
+    <t>juízo criminal</t>
+  </si>
+  <si>
+    <t>eis informado</t>
+  </si>
+  <si>
+    <t>fundamentos insubsistência</t>
+  </si>
+  <si>
+    <t>liminar espécie</t>
+  </si>
+  <si>
+    <t>efêmero</t>
+  </si>
+  <si>
+    <t>deferida assessoria</t>
+  </si>
+  <si>
+    <t>deferi pedido</t>
+  </si>
+  <si>
+    <t>decretada desfavor</t>
+  </si>
+  <si>
     <t>decisão proferida</t>
   </si>
   <si>
-    <t>aumento</t>
-  </si>
-  <si>
-    <t>xliii</t>
-  </si>
-  <si>
-    <t>concessão</t>
-  </si>
-  <si>
-    <t>ordem prisão</t>
-  </si>
-  <si>
-    <t>justiça indeferiu</t>
-  </si>
-  <si>
-    <t>julgado turma</t>
-  </si>
-  <si>
-    <t>arquivado</t>
-  </si>
-  <si>
-    <t>enunciado súmula</t>
-  </si>
-  <si>
-    <t>deferida</t>
-  </si>
-  <si>
-    <t>senha relatório</t>
-  </si>
-  <si>
-    <t>concessão ordem</t>
-  </si>
-  <si>
-    <t>outro motivo</t>
-  </si>
-  <si>
-    <t>liberdade provisória</t>
-  </si>
-  <si>
-    <t>assessoria</t>
-  </si>
-  <si>
-    <t>implicou deferimento</t>
-  </si>
-  <si>
-    <t>deferido</t>
-  </si>
-  <si>
-    <t>liminar espécie</t>
-  </si>
-  <si>
-    <t>stj indeferiu</t>
-  </si>
-  <si>
-    <t>liminar hc</t>
-  </si>
-  <si>
-    <t>deferi</t>
-  </si>
-  <si>
-    <t>relatório http</t>
-  </si>
-  <si>
-    <t>restritiva direitos</t>
-  </si>
-  <si>
-    <t>manifesta ilegalidade</t>
-  </si>
-  <si>
-    <t>opina deferimento</t>
-  </si>
-  <si>
-    <t>restritiva</t>
-  </si>
-  <si>
-    <t>informado</t>
-  </si>
-  <si>
-    <t>http sob</t>
-  </si>
-  <si>
-    <t>inconstitucional</t>
-  </si>
-  <si>
-    <t>provisória formulado</t>
-  </si>
-  <si>
-    <t>cautelar pois</t>
-  </si>
-  <si>
-    <t>proferida ministro</t>
-  </si>
-  <si>
-    <t>preventiva fundamentos</t>
-  </si>
-  <si>
-    <t>tutela cautelar</t>
-  </si>
-  <si>
-    <t>fundamentos insubsistência</t>
-  </si>
-  <si>
-    <t>liminar suspender</t>
-  </si>
-  <si>
-    <t>lxi</t>
-  </si>
-  <si>
-    <t>opinou concessão</t>
-  </si>
-  <si>
-    <t>arquivado definitivo</t>
-  </si>
-  <si>
-    <t>república concessão</t>
-  </si>
-  <si>
-    <t>gabinete prestou</t>
-  </si>
-  <si>
-    <t>formalizado ato</t>
-  </si>
-  <si>
-    <t>deferimento liminar</t>
-  </si>
-  <si>
-    <t>deferida assessoria</t>
-  </si>
-  <si>
-    <t>deferi pedido</t>
-  </si>
-  <si>
-    <t>sobrestamento</t>
+    <t>decisão implicou</t>
   </si>
   <si>
     <t>código senha</t>
   </si>
   <si>
+    <t>paulo indeferiu</t>
+  </si>
+  <si>
+    <t>precário</t>
+  </si>
+  <si>
+    <t>precário efêmero</t>
+  </si>
+  <si>
     <t>contornos impetração</t>
   </si>
   <si>
-    <t>desta suprema</t>
-  </si>
-  <si>
-    <t>definitivo após</t>
-  </si>
-  <si>
-    <t>efêmero</t>
-  </si>
-  <si>
-    <t>resumida prisão</t>
-  </si>
-  <si>
-    <t>senha primeira</t>
-  </si>
-  <si>
-    <t>benefício liberdade</t>
-  </si>
-  <si>
-    <t>ficou</t>
-  </si>
-  <si>
-    <t>flagrante tráfico</t>
-  </si>
-  <si>
-    <t>sob código</t>
-  </si>
-  <si>
-    <t>precário</t>
-  </si>
-  <si>
-    <t>pertence grifei</t>
-  </si>
-  <si>
-    <t>precário efêmero</t>
-  </si>
-  <si>
-    <t>suspender efeitos</t>
-  </si>
-  <si>
-    <t>sistema jurídico</t>
-  </si>
-  <si>
-    <t>senha</t>
-  </si>
-  <si>
-    <t>princípio liberdade</t>
-  </si>
-  <si>
-    <t>rtj rel</t>
-  </si>
-  <si>
-    <t>processo formalizado</t>
-  </si>
-  <si>
-    <t>revelou contornos</t>
-  </si>
-  <si>
-    <t>punir</t>
-  </si>
-  <si>
-    <t>suspender</t>
-  </si>
-  <si>
-    <t>paulo indeferiu</t>
-  </si>
-  <si>
-    <t>resumida</t>
-  </si>
-  <si>
-    <t>análise pedido</t>
-  </si>
-  <si>
-    <t>mendes hc</t>
-  </si>
-  <si>
-    <t>liminar deferida</t>
-  </si>
-  <si>
-    <t>art lvii</t>
-  </si>
-  <si>
-    <t>art lxi</t>
-  </si>
-  <si>
-    <t>assessoria prestou</t>
-  </si>
-  <si>
-    <t>assim resumida</t>
-  </si>
-  <si>
-    <t>assim revelou</t>
-  </si>
-  <si>
-    <t>aurélio decisão</t>
-  </si>
-  <si>
-    <t>campo precário</t>
-  </si>
-  <si>
-    <t>condenação penal</t>
-  </si>
-  <si>
-    <t>constitucional cf</t>
-  </si>
-  <si>
-    <t>defiro</t>
-  </si>
-  <si>
-    <t>deserção</t>
-  </si>
-  <si>
-    <t>efeitos ordem</t>
-  </si>
-  <si>
-    <t>eis informado</t>
-  </si>
-  <si>
-    <t>espécie ficou</t>
-  </si>
-  <si>
-    <t>fiança</t>
-  </si>
-  <si>
-    <t>ficou assim</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>impetração eis</t>
-  </si>
-  <si>
-    <t>inciso xliii</t>
-  </si>
-  <si>
-    <t>indefiro pedido</t>
-  </si>
-  <si>
-    <t>infligir</t>
-  </si>
-  <si>
-    <t>infligir punição</t>
-  </si>
-  <si>
-    <t>informado análise</t>
-  </si>
-  <si>
-    <t>instituto prisão</t>
-  </si>
-  <si>
-    <t>irrecorrível</t>
-  </si>
-  <si>
-    <t>indiciado réu</t>
+    <t>óbice previsto</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -704,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -712,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
+        <v>0.046875</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -720,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.03</v>
+        <v>0.046875</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -736,7 +736,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -744,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -752,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -760,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -768,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -784,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.02</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -808,7 +808,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -816,7 +816,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -832,7 +832,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -840,7 +840,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -848,7 +848,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -856,7 +856,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -864,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -872,7 +872,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -880,7 +880,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -888,7 +888,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -896,7 +896,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -904,7 +904,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.02</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -912,7 +912,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -920,7 +920,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -928,7 +928,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -936,7 +936,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -944,7 +944,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -952,7 +952,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -960,7 +960,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -968,7 +968,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -976,7 +976,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -984,7 +984,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -992,7 +992,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1000,7 +1000,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1008,7 +1008,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1016,7 +1016,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1024,7 +1024,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1032,7 +1032,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1040,7 +1040,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.01</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1048,7 +1048,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1056,7 +1056,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1064,7 +1064,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1072,7 +1072,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1080,7 +1080,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1088,7 +1088,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1096,7 +1096,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1104,7 +1104,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1112,7 +1112,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1120,7 +1120,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1128,7 +1128,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1136,7 +1136,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">

</xml_diff>